<commit_message>
add: checklist | fix: TestDocumentation
</commit_message>
<xml_diff>
--- a/TestDocumentation/TestDocumentation.xlsx
+++ b/TestDocumentation/TestDocumentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA_Slack\TestDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2098A9E6-1DAF-4774-A606-2E2D1B2C50D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22F2C26-D226-423B-82C3-A74E1C26A077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>Ввести 10 латинских букв</t>
   </si>
   <si>
-    <t>Остальный поля заполнены валидными данными</t>
-  </si>
-  <si>
     <t>Nikitaqaqa</t>
   </si>
   <si>
@@ -277,9 +274,6 @@
   </si>
   <si>
     <t>Ввести валидный Name</t>
-  </si>
-  <si>
-    <t>Остальные поля оставить пыстыми</t>
   </si>
   <si>
     <t>Ввести валидный Name и Surname</t>
@@ -893,14 +887,6 @@
   </si>
   <si>
     <t>Improvement</t>
-  </si>
-  <si>
-    <t>1. Добавить в поле "Пароль" скрыть/открыть пароль
-2. Добавить проверку надожности паролья
-3. Добавить поле "Подтвердить пароль"
-4. Для всех полей добавить подсказку о валидных и невалидных символах
-5. Привести заголовки полей к единому стилю
-6. Привести placeholder полях к единому стилю</t>
   </si>
   <si>
     <r>
@@ -914,6 +900,20 @@
       </rPr>
       <t xml:space="preserve"> - тест-кейсы с Name</t>
     </r>
+  </si>
+  <si>
+    <t>Остальные поля оставить пустыми</t>
+  </si>
+  <si>
+    <t>Остальные поля заполнены валидными данными</t>
+  </si>
+  <si>
+    <t>1. Добавить в поле "Пароль" скрыть/открыть пароль
+2. Добавить проверку надежности пароля
+3. Добавить поле "Подтвердить пароль"
+4. Для всех полей добавить подсказку о валидных и невалидных символах
+5. Привести заголовки полей к единому стилю
+6. Привести placeholder полей к единому стилю</t>
   </si>
 </sst>
 </file>
@@ -1654,7 +1654,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J100" sqref="J100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1726,17 +1726,17 @@
         <v>9</v>
       </c>
       <c r="C4" s="38" t="s">
+        <v>282</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -1745,18 +1745,18 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="4"/>
     </row>
@@ -1765,23 +1765,23 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1789,23 +1789,23 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1813,23 +1813,23 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1837,23 +1837,23 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1861,18 +1861,18 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="30"/>
       <c r="D10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H10" s="4"/>
     </row>
@@ -1881,18 +1881,18 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="30"/>
       <c r="D11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="4"/>
     </row>
@@ -1901,18 +1901,18 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="30"/>
       <c r="D12" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" s="4"/>
     </row>
@@ -1921,18 +1921,18 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" s="4"/>
     </row>
@@ -1941,18 +1941,18 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="8">
         <v>12345</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H14" s="4"/>
     </row>
@@ -1961,23 +1961,23 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1985,18 +1985,18 @@
         <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" s="4"/>
     </row>
@@ -2005,18 +2005,18 @@
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" s="4"/>
     </row>
@@ -2025,16 +2025,16 @@
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H18" s="4"/>
     </row>
@@ -2043,23 +2043,23 @@
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2067,18 +2067,18 @@
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="30"/>
       <c r="D20" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H20" s="4"/>
     </row>
@@ -2087,18 +2087,18 @@
         <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H21" s="4"/>
     </row>
@@ -2107,16 +2107,16 @@
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H22" s="4"/>
     </row>
@@ -2125,16 +2125,16 @@
         <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H23" s="4"/>
     </row>
@@ -2143,18 +2143,18 @@
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H24" s="4"/>
     </row>
@@ -2163,23 +2163,23 @@
         <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2187,23 +2187,23 @@
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="30"/>
       <c r="D26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2211,18 +2211,18 @@
         <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H27" s="4"/>
     </row>
@@ -2231,23 +2231,23 @@
         <v>25</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2255,23 +2255,23 @@
         <v>26</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="30"/>
       <c r="D29" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="G29" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2279,17 +2279,17 @@
         <v>27</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
@@ -2299,16 +2299,16 @@
         <v>28</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="30"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H31" s="4"/>
     </row>
@@ -2317,16 +2317,16 @@
         <v>29</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H32" s="4"/>
     </row>
@@ -2335,23 +2335,23 @@
         <v>30</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="31"/>
       <c r="D33" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2359,20 +2359,20 @@
         <v>31</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>83</v>
+        <v>281</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H34" s="4"/>
     </row>
@@ -2381,23 +2381,23 @@
         <v>32</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C35" s="30"/>
       <c r="D35" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2405,18 +2405,18 @@
         <v>33</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C36" s="30"/>
       <c r="D36" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H36" s="4"/>
     </row>
@@ -2425,18 +2425,18 @@
         <v>34</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C37" s="30"/>
       <c r="D37" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H37" s="4"/>
     </row>
@@ -2445,23 +2445,23 @@
         <v>35</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C38" s="30"/>
       <c r="D38" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -2469,23 +2469,23 @@
         <v>36</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C39" s="30"/>
       <c r="D39" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2493,28 +2493,28 @@
         <v>37</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C40" s="31"/>
       <c r="D40" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="39" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B41" s="33"/>
       <c r="C41" s="33"/>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="42" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="32" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B42" s="33"/>
       <c r="C42" s="33"/>
@@ -2541,20 +2541,20 @@
         <v>38</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>10</v>
+        <v>282</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H43" s="4"/>
     </row>
@@ -2563,23 +2563,23 @@
         <v>39</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C44" s="30"/>
       <c r="D44" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2587,18 +2587,18 @@
         <v>40</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C45" s="30"/>
       <c r="D45" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H45" s="4"/>
     </row>
@@ -2607,18 +2607,18 @@
         <v>41</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C46" s="30"/>
       <c r="D46" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H46" s="4"/>
     </row>
@@ -2627,18 +2627,18 @@
         <v>42</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C47" s="30"/>
       <c r="D47" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H47" s="4"/>
     </row>
@@ -2647,18 +2647,18 @@
         <v>43</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C48" s="30"/>
       <c r="D48" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H48" s="4"/>
     </row>
@@ -2667,23 +2667,23 @@
         <v>44</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C49" s="30"/>
       <c r="D49" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2691,18 +2691,18 @@
         <v>45</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C50" s="30"/>
       <c r="D50" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H50" s="4"/>
     </row>
@@ -2711,23 +2711,23 @@
         <v>46</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C51" s="30"/>
       <c r="D51" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2735,18 +2735,18 @@
         <v>47</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C52" s="30"/>
       <c r="D52" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H52" s="4"/>
     </row>
@@ -2755,18 +2755,18 @@
         <v>48</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C53" s="30"/>
       <c r="D53" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H53" s="4"/>
     </row>
@@ -2775,18 +2775,18 @@
         <v>49</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C54" s="30"/>
       <c r="D54" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H54" s="4"/>
     </row>
@@ -2795,18 +2795,18 @@
         <v>50</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C55" s="30"/>
       <c r="D55" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H55" s="4"/>
     </row>
@@ -2815,23 +2815,23 @@
         <v>51</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C56" s="30"/>
       <c r="D56" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2839,18 +2839,18 @@
         <v>52</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C57" s="30"/>
       <c r="D57" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H57" s="4"/>
     </row>
@@ -2859,23 +2859,23 @@
         <v>53</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C58" s="30"/>
       <c r="D58" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2883,18 +2883,18 @@
         <v>54</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C59" s="30"/>
       <c r="D59" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H59" s="4"/>
     </row>
@@ -2903,18 +2903,18 @@
         <v>55</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C60" s="30"/>
       <c r="D60" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H60" s="4"/>
     </row>
@@ -2923,18 +2923,18 @@
         <v>56</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C61" s="30"/>
       <c r="D61" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F61" s="4"/>
       <c r="G61" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H61" s="4"/>
     </row>
@@ -2943,18 +2943,18 @@
         <v>57</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C62" s="30"/>
       <c r="D62" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H62" s="4"/>
     </row>
@@ -2963,23 +2963,23 @@
         <v>58</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C63" s="30"/>
       <c r="D63" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2987,18 +2987,18 @@
         <v>59</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C64" s="30"/>
       <c r="D64" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H64" s="4"/>
     </row>
@@ -3007,18 +3007,18 @@
         <v>60</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C65" s="30"/>
       <c r="D65" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H65" s="4"/>
     </row>
@@ -3027,23 +3027,23 @@
         <v>61</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C66" s="30"/>
       <c r="D66" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3051,18 +3051,18 @@
         <v>62</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C67" s="30"/>
       <c r="D67" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F67" s="4"/>
       <c r="G67" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H67" s="4"/>
     </row>
@@ -3071,18 +3071,18 @@
         <v>63</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C68" s="30"/>
       <c r="D68" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F68" s="4"/>
       <c r="G68" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H68" s="4"/>
     </row>
@@ -3091,23 +3091,23 @@
         <v>64</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C69" s="30"/>
       <c r="D69" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3115,18 +3115,18 @@
         <v>65</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C70" s="30"/>
       <c r="D70" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H70" s="4"/>
     </row>
@@ -3135,23 +3135,23 @@
         <v>66</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C71" s="30"/>
       <c r="D71" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3159,18 +3159,18 @@
         <v>67</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C72" s="30"/>
       <c r="D72" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F72" s="4"/>
       <c r="G72" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H72" s="4"/>
     </row>
@@ -3179,18 +3179,18 @@
         <v>68</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C73" s="30"/>
       <c r="D73" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F73" s="4"/>
       <c r="G73" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H73" s="4"/>
     </row>
@@ -3199,21 +3199,21 @@
         <v>69</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C74" s="30"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3221,23 +3221,23 @@
         <v>70</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C75" s="30"/>
       <c r="D75" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3245,18 +3245,18 @@
         <v>71</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C76" s="30"/>
       <c r="D76" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F76" s="4"/>
       <c r="G76" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H76" s="4"/>
     </row>
@@ -3265,18 +3265,18 @@
         <v>72</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C77" s="30"/>
       <c r="D77" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F77" s="4"/>
       <c r="G77" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H77" s="4"/>
     </row>
@@ -3285,16 +3285,16 @@
         <v>73</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C78" s="30"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F78" s="4"/>
       <c r="G78" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H78" s="4"/>
     </row>
@@ -3303,16 +3303,16 @@
         <v>74</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C79" s="30"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H79" s="4"/>
     </row>
@@ -3321,23 +3321,23 @@
         <v>75</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C80" s="30"/>
       <c r="D80" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3345,18 +3345,18 @@
         <v>76</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C81" s="30"/>
       <c r="D81" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F81" s="4"/>
       <c r="G81" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H81" s="4"/>
     </row>
@@ -3365,23 +3365,23 @@
         <v>77</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C82" s="30"/>
       <c r="D82" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3389,23 +3389,23 @@
         <v>78</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C83" s="30"/>
       <c r="D83" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -3413,23 +3413,23 @@
         <v>79</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C84" s="30"/>
       <c r="D84" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3437,23 +3437,23 @@
         <v>80</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C85" s="30"/>
       <c r="D85" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H85" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F85" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="G85" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H85" s="4" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3461,23 +3461,23 @@
         <v>81</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C86" s="30"/>
       <c r="D86" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3485,16 +3485,16 @@
         <v>82</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C87" s="30"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F87" s="4"/>
       <c r="G87" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H87" s="4"/>
     </row>
@@ -3503,16 +3503,16 @@
         <v>83</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C88" s="30"/>
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F88" s="4"/>
       <c r="G88" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H88" s="4"/>
     </row>
@@ -3521,28 +3521,28 @@
         <v>84</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C89" s="31"/>
       <c r="D89" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="32" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B90" s="33"/>
       <c r="C90" s="33"/>
@@ -3557,25 +3557,25 @@
         <v>85</v>
       </c>
       <c r="B91" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C91" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E91" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C91" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D91" s="4" t="s">
+      <c r="F91" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H91" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="E91" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="F91" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G91" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H91" s="4" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3583,18 +3583,18 @@
         <v>86</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C92" s="30"/>
       <c r="D92" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F92" s="4"/>
       <c r="G92" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H92" s="4"/>
     </row>
@@ -3603,18 +3603,18 @@
         <v>87</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C93" s="30"/>
       <c r="D93" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F93" s="4"/>
       <c r="G93" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H93" s="4"/>
     </row>
@@ -3623,18 +3623,18 @@
         <v>88</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C94" s="30"/>
       <c r="D94" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F94" s="4"/>
       <c r="G94" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H94" s="4"/>
     </row>
@@ -3643,18 +3643,18 @@
         <v>89</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C95" s="30"/>
       <c r="D95" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F95" s="4"/>
       <c r="G95" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H95" s="4"/>
     </row>
@@ -3663,23 +3663,23 @@
         <v>90</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C96" s="30"/>
       <c r="D96" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G96" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H96" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3687,23 +3687,23 @@
         <v>91</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C97" s="30"/>
       <c r="D97" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H97" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3711,23 +3711,23 @@
         <v>92</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C98" s="30"/>
       <c r="D98" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G98" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H98" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3735,23 +3735,23 @@
         <v>93</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C99" s="30"/>
       <c r="D99" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H99" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3759,23 +3759,23 @@
         <v>94</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C100" s="30"/>
       <c r="D100" s="4">
         <v>12345678</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H100" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3783,23 +3783,23 @@
         <v>95</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C101" s="30"/>
       <c r="D101" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H101" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3807,23 +3807,23 @@
         <v>96</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C102" s="30"/>
       <c r="D102" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G102" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H102" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3831,21 +3831,21 @@
         <v>97</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C103" s="30"/>
       <c r="D103" s="4"/>
       <c r="E103" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G103" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H103" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3853,23 +3853,23 @@
         <v>98</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C104" s="30"/>
       <c r="D104" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G104" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H104" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3877,23 +3877,23 @@
         <v>99</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C105" s="30"/>
       <c r="D105" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G105" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H105" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3901,23 +3901,23 @@
         <v>100</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C106" s="30"/>
       <c r="D106" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G106" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H106" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -3925,23 +3925,23 @@
         <v>101</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C107" s="30"/>
       <c r="D107" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G107" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H107" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3949,18 +3949,18 @@
         <v>102</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C108" s="30"/>
       <c r="D108" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F108" s="4"/>
       <c r="G108" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H108" s="4"/>
     </row>
@@ -3969,18 +3969,18 @@
         <v>103</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C109" s="30"/>
       <c r="D109" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F109" s="4"/>
       <c r="G109" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H109" s="4"/>
     </row>
@@ -3989,18 +3989,18 @@
         <v>104</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C110" s="30"/>
       <c r="D110" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E110" s="4" t="s">
         <v>247</v>
-      </c>
-      <c r="E110" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="F110" s="4"/>
       <c r="G110" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H110" s="4"/>
     </row>
@@ -4009,16 +4009,16 @@
         <v>105</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C111" s="30"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F111" s="4"/>
       <c r="G111" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H111" s="4"/>
     </row>
@@ -4027,16 +4027,16 @@
         <v>106</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C112" s="30"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F112" s="4"/>
       <c r="G112" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H112" s="4"/>
     </row>
@@ -4045,16 +4045,16 @@
         <v>107</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C113" s="30"/>
       <c r="D113" s="4"/>
       <c r="E113" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F113" s="10"/>
       <c r="G113" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H113" s="4"/>
     </row>
@@ -4063,16 +4063,16 @@
         <v>108</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C114" s="30"/>
       <c r="D114" s="2"/>
       <c r="E114" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F114" s="10"/>
       <c r="G114" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H114" s="4"/>
     </row>
@@ -4081,23 +4081,23 @@
         <v>109</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C115" s="31"/>
       <c r="D115" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G115" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H115" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5094,10 +5094,10 @@
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -5110,7 +5110,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -5120,10 +5120,10 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -5133,10 +5133,10 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -5146,10 +5146,10 @@
     </row>
     <row r="6" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -5162,7 +5162,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -5172,10 +5172,10 @@
     </row>
     <row r="8" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -5188,7 +5188,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -5201,7 +5201,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -5211,7 +5211,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="1"/>
@@ -5240,10 +5240,10 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -5256,7 +5256,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -5266,10 +5266,10 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -5279,10 +5279,10 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -5292,10 +5292,10 @@
     </row>
     <row r="18" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -5308,7 +5308,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -5318,10 +5318,10 @@
     </row>
     <row r="20" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -5334,7 +5334,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -5347,7 +5347,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -5357,7 +5357,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="1"/>
@@ -5386,10 +5386,10 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -5402,7 +5402,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -5412,10 +5412,10 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -5425,10 +5425,10 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -5438,10 +5438,10 @@
     </row>
     <row r="30" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -5454,7 +5454,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -5464,10 +5464,10 @@
     </row>
     <row r="32" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -5480,7 +5480,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -5493,7 +5493,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -5503,7 +5503,7 @@
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B35" s="16"/>
       <c r="C35" s="1"/>
@@ -5532,10 +5532,10 @@
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -5548,7 +5548,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -5558,10 +5558,10 @@
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -5571,10 +5571,10 @@
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -5584,10 +5584,10 @@
     </row>
     <row r="42" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -5600,7 +5600,7 @@
         <v>2</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -5610,10 +5610,10 @@
     </row>
     <row r="44" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -5626,7 +5626,7 @@
         <v>5</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -5639,7 +5639,7 @@
         <v>4</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -5649,7 +5649,7 @@
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B47" s="16"/>
       <c r="C47" s="1"/>
@@ -5678,10 +5678,10 @@
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -5694,7 +5694,7 @@
         <v>1</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -5704,10 +5704,10 @@
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -5717,10 +5717,10 @@
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -5730,10 +5730,10 @@
     </row>
     <row r="54" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -5746,7 +5746,7 @@
         <v>2</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -5756,10 +5756,10 @@
     </row>
     <row r="56" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -5772,7 +5772,7 @@
         <v>5</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -5785,7 +5785,7 @@
         <v>4</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -5795,7 +5795,7 @@
     </row>
     <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B59" s="16"/>
       <c r="C59" s="1"/>
@@ -5824,10 +5824,10 @@
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -5840,7 +5840,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -5850,26 +5850,26 @@
     </row>
     <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5877,15 +5877,15 @@
         <v>2</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5893,7 +5893,7 @@
         <v>5</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5901,12 +5901,12 @@
         <v>4</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B71" s="16"/>
     </row>
@@ -5918,10 +5918,10 @@
     </row>
     <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5929,31 +5929,31 @@
         <v>1</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -5961,15 +5961,15 @@
         <v>2</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5977,7 +5977,7 @@
         <v>5</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5985,12 +5985,12 @@
         <v>4</v>
       </c>
       <c r="B82" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B83" s="16"/>
     </row>
@@ -6002,10 +6002,10 @@
     </row>
     <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6013,31 +6013,31 @@
         <v>1</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6045,15 +6045,15 @@
         <v>2</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6061,7 +6061,7 @@
         <v>5</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6069,12 +6069,12 @@
         <v>4</v>
       </c>
       <c r="B94" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B95" s="16"/>
     </row>
@@ -6086,10 +6086,10 @@
     </row>
     <row r="98" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B98" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6097,31 +6097,31 @@
         <v>1</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B101" s="15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -6129,15 +6129,15 @@
         <v>2</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6145,7 +6145,7 @@
         <v>5</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6153,12 +6153,12 @@
         <v>4</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B107" s="16"/>
     </row>
@@ -7263,7 +7263,7 @@
   <customSheetViews>
     <customSheetView guid="{0B523258-5331-49A5-8E12-7693DC3B142F}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:B11" xr:uid="{F6689995-DFE3-46B6-A4DE-CB58E074F4C0}"/>
+      <autoFilter ref="A2:B11" xr:uid="{42C76EB5-83CE-421F-ACC2-328E68B003D7}"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -7279,7 +7279,7 @@
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A3" sqref="A3:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7293,12 +7293,12 @@
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add: test documentation files
</commit_message>
<xml_diff>
--- a/TestDocumentation/TestDocumentation.xlsx
+++ b/TestDocumentation/TestDocumentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA_Slack\TestDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22F2C26-D226-423B-82C3-A74E1C26A077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A298E7B0-0D85-4046-B786-1544DBEFF7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -897,6 +897,8 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
       </rPr>
       <t xml:space="preserve"> - тест-кейсы с Name</t>
     </r>
@@ -931,32 +933,44 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1400,15 +1414,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1432,6 +1437,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1653,8 +1667,8 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J100" sqref="J100"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1680,43 +1694,43 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:8" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="40" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="37"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -1725,7 +1739,7 @@
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="35" t="s">
         <v>282</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1747,7 +1761,7 @@
       <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="30"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1767,7 +1781,7 @@
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1791,7 +1805,7 @@
       <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="30"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1815,7 +1829,7 @@
       <c r="B8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="4" t="s">
         <v>24</v>
       </c>
@@ -1839,7 +1853,7 @@
       <c r="B9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="30"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
@@ -1863,7 +1877,7 @@
       <c r="B10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="30"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="4" t="s">
         <v>30</v>
       </c>
@@ -1883,7 +1897,7 @@
       <c r="B11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="30"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
@@ -1903,7 +1917,7 @@
       <c r="B12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="4" t="s">
         <v>34</v>
       </c>
@@ -1923,7 +1937,7 @@
       <c r="B13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="30"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="4" t="s">
         <v>36</v>
       </c>
@@ -1943,7 +1957,7 @@
       <c r="B14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="30"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="8">
         <v>12345</v>
       </c>
@@ -1963,7 +1977,7 @@
       <c r="B15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="30"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="4" t="s">
         <v>39</v>
       </c>
@@ -1987,7 +2001,7 @@
       <c r="B16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="30"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="4" t="s">
         <v>42</v>
       </c>
@@ -2007,7 +2021,7 @@
       <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="30"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="4" t="s">
         <v>44</v>
       </c>
@@ -2027,7 +2041,7 @@
       <c r="B18" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="30"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
         <v>15</v>
@@ -2045,7 +2059,7 @@
       <c r="B19" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="30"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="4" t="s">
         <v>47</v>
       </c>
@@ -2069,7 +2083,7 @@
       <c r="B20" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="30"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="4" t="s">
         <v>42</v>
       </c>
@@ -2089,7 +2103,7 @@
       <c r="B21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="30"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="4" t="s">
         <v>42</v>
       </c>
@@ -2109,7 +2123,7 @@
       <c r="B22" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="30"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
         <v>52</v>
@@ -2127,7 +2141,7 @@
       <c r="B23" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="30"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
         <v>54</v>
@@ -2145,7 +2159,7 @@
       <c r="B24" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="30"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="4" t="s">
         <v>42</v>
       </c>
@@ -2165,7 +2179,7 @@
       <c r="B25" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="30"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="4" t="s">
         <v>57</v>
       </c>
@@ -2189,7 +2203,7 @@
       <c r="B26" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="30"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="4" t="s">
         <v>60</v>
       </c>
@@ -2213,7 +2227,7 @@
       <c r="B27" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="30"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="4" t="s">
         <v>42</v>
       </c>
@@ -2233,7 +2247,7 @@
       <c r="B28" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="30"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="4" t="s">
         <v>65</v>
       </c>
@@ -2257,7 +2271,7 @@
       <c r="B29" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="30"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="4" t="s">
         <v>68</v>
       </c>
@@ -2281,7 +2295,7 @@
       <c r="B30" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="30"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="4" t="s">
         <v>73</v>
       </c>
@@ -2301,7 +2315,7 @@
       <c r="B31" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="30"/>
+      <c r="C31" s="27"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
         <v>75</v>
@@ -2319,7 +2333,7 @@
       <c r="B32" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="30"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
         <v>77</v>
@@ -2337,7 +2351,7 @@
       <c r="B33" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="31"/>
+      <c r="C33" s="28"/>
       <c r="D33" s="4" t="s">
         <v>79</v>
       </c>
@@ -2361,7 +2375,7 @@
       <c r="B34" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="26" t="s">
         <v>281</v>
       </c>
       <c r="D34" s="4" t="s">
@@ -2383,7 +2397,7 @@
       <c r="B35" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="30"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="4" t="s">
         <v>83</v>
       </c>
@@ -2407,7 +2421,7 @@
       <c r="B36" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="30"/>
+      <c r="C36" s="27"/>
       <c r="D36" s="4" t="s">
         <v>86</v>
       </c>
@@ -2427,7 +2441,7 @@
       <c r="B37" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C37" s="30"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="4" t="s">
         <v>88</v>
       </c>
@@ -2447,7 +2461,7 @@
       <c r="B38" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C38" s="30"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="4" t="s">
         <v>90</v>
       </c>
@@ -2471,7 +2485,7 @@
       <c r="B39" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="30"/>
+      <c r="C39" s="27"/>
       <c r="D39" s="4" t="s">
         <v>93</v>
       </c>
@@ -2495,7 +2509,7 @@
       <c r="B40" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C40" s="31"/>
+      <c r="C40" s="28"/>
       <c r="D40" s="4" t="s">
         <v>96</v>
       </c>
@@ -2513,28 +2527,28 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="36" t="s">
         <v>280</v>
       </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="34"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="31"/>
     </row>
     <row r="42" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B42" s="33"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="34"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="31"/>
     </row>
     <row r="43" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
@@ -2543,7 +2557,7 @@
       <c r="B43" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C43" s="29" t="s">
+      <c r="C43" s="26" t="s">
         <v>282</v>
       </c>
       <c r="D43" s="4" t="s">
@@ -2565,7 +2579,7 @@
       <c r="B44" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="30"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="4" t="s">
         <v>102</v>
       </c>
@@ -2589,7 +2603,7 @@
       <c r="B45" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C45" s="30"/>
+      <c r="C45" s="27"/>
       <c r="D45" s="4" t="s">
         <v>105</v>
       </c>
@@ -2609,7 +2623,7 @@
       <c r="B46" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C46" s="30"/>
+      <c r="C46" s="27"/>
       <c r="D46" s="4" t="s">
         <v>107</v>
       </c>
@@ -2629,7 +2643,7 @@
       <c r="B47" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C47" s="30"/>
+      <c r="C47" s="27"/>
       <c r="D47" s="4" t="s">
         <v>109</v>
       </c>
@@ -2649,7 +2663,7 @@
       <c r="B48" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C48" s="30"/>
+      <c r="C48" s="27"/>
       <c r="D48" s="4" t="s">
         <v>111</v>
       </c>
@@ -2669,7 +2683,7 @@
       <c r="B49" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C49" s="30"/>
+      <c r="C49" s="27"/>
       <c r="D49" s="4" t="s">
         <v>113</v>
       </c>
@@ -2693,7 +2707,7 @@
       <c r="B50" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C50" s="30"/>
+      <c r="C50" s="27"/>
       <c r="D50" s="4" t="s">
         <v>116</v>
       </c>
@@ -2713,7 +2727,7 @@
       <c r="B51" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C51" s="30"/>
+      <c r="C51" s="27"/>
       <c r="D51" s="4" t="s">
         <v>118</v>
       </c>
@@ -2737,7 +2751,7 @@
       <c r="B52" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C52" s="30"/>
+      <c r="C52" s="27"/>
       <c r="D52" s="4" t="s">
         <v>121</v>
       </c>
@@ -2757,7 +2771,7 @@
       <c r="B53" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C53" s="30"/>
+      <c r="C53" s="27"/>
       <c r="D53" s="4" t="s">
         <v>123</v>
       </c>
@@ -2777,7 +2791,7 @@
       <c r="B54" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C54" s="30"/>
+      <c r="C54" s="27"/>
       <c r="D54" s="4" t="s">
         <v>125</v>
       </c>
@@ -2797,7 +2811,7 @@
       <c r="B55" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C55" s="30"/>
+      <c r="C55" s="27"/>
       <c r="D55" s="4" t="s">
         <v>127</v>
       </c>
@@ -2817,7 +2831,7 @@
       <c r="B56" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C56" s="30"/>
+      <c r="C56" s="27"/>
       <c r="D56" s="4" t="s">
         <v>129</v>
       </c>
@@ -2841,7 +2855,7 @@
       <c r="B57" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C57" s="30"/>
+      <c r="C57" s="27"/>
       <c r="D57" s="4" t="s">
         <v>132</v>
       </c>
@@ -2861,7 +2875,7 @@
       <c r="B58" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C58" s="30"/>
+      <c r="C58" s="27"/>
       <c r="D58" s="4" t="s">
         <v>134</v>
       </c>
@@ -2885,7 +2899,7 @@
       <c r="B59" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C59" s="30"/>
+      <c r="C59" s="27"/>
       <c r="D59" s="4" t="s">
         <v>137</v>
       </c>
@@ -2905,7 +2919,7 @@
       <c r="B60" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C60" s="30"/>
+      <c r="C60" s="27"/>
       <c r="D60" s="4" t="s">
         <v>107</v>
       </c>
@@ -2925,7 +2939,7 @@
       <c r="B61" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C61" s="30"/>
+      <c r="C61" s="27"/>
       <c r="D61" s="4" t="s">
         <v>140</v>
       </c>
@@ -2945,7 +2959,7 @@
       <c r="B62" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C62" s="30"/>
+      <c r="C62" s="27"/>
       <c r="D62" s="4" t="s">
         <v>142</v>
       </c>
@@ -2965,7 +2979,7 @@
       <c r="B63" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C63" s="30"/>
+      <c r="C63" s="27"/>
       <c r="D63" s="4" t="s">
         <v>144</v>
       </c>
@@ -2989,7 +3003,7 @@
       <c r="B64" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C64" s="30"/>
+      <c r="C64" s="27"/>
       <c r="D64" s="4" t="s">
         <v>147</v>
       </c>
@@ -3009,7 +3023,7 @@
       <c r="B65" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C65" s="30"/>
+      <c r="C65" s="27"/>
       <c r="D65" s="4" t="s">
         <v>149</v>
       </c>
@@ -3029,7 +3043,7 @@
       <c r="B66" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C66" s="30"/>
+      <c r="C66" s="27"/>
       <c r="D66" s="4" t="s">
         <v>151</v>
       </c>
@@ -3053,7 +3067,7 @@
       <c r="B67" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C67" s="30"/>
+      <c r="C67" s="27"/>
       <c r="D67" s="4" t="s">
         <v>154</v>
       </c>
@@ -3073,7 +3087,7 @@
       <c r="B68" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C68" s="30"/>
+      <c r="C68" s="27"/>
       <c r="D68" s="4" t="s">
         <v>156</v>
       </c>
@@ -3093,7 +3107,7 @@
       <c r="B69" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C69" s="30"/>
+      <c r="C69" s="27"/>
       <c r="D69" s="4" t="s">
         <v>158</v>
       </c>
@@ -3117,7 +3131,7 @@
       <c r="B70" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C70" s="30"/>
+      <c r="C70" s="27"/>
       <c r="D70" s="4" t="s">
         <v>161</v>
       </c>
@@ -3137,7 +3151,7 @@
       <c r="B71" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C71" s="30"/>
+      <c r="C71" s="27"/>
       <c r="D71" s="4" t="s">
         <v>163</v>
       </c>
@@ -3161,7 +3175,7 @@
       <c r="B72" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C72" s="30"/>
+      <c r="C72" s="27"/>
       <c r="D72" s="4" t="s">
         <v>100</v>
       </c>
@@ -3181,7 +3195,7 @@
       <c r="B73" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C73" s="30"/>
+      <c r="C73" s="27"/>
       <c r="D73" s="4" t="s">
         <v>167</v>
       </c>
@@ -3201,7 +3215,7 @@
       <c r="B74" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C74" s="30"/>
+      <c r="C74" s="27"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
         <v>15</v>
@@ -3223,7 +3237,7 @@
       <c r="B75" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C75" s="30"/>
+      <c r="C75" s="27"/>
       <c r="D75" s="4" t="s">
         <v>170</v>
       </c>
@@ -3247,7 +3261,7 @@
       <c r="B76" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C76" s="30"/>
+      <c r="C76" s="27"/>
       <c r="D76" s="4" t="s">
         <v>100</v>
       </c>
@@ -3267,7 +3281,7 @@
       <c r="B77" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C77" s="30"/>
+      <c r="C77" s="27"/>
       <c r="D77" s="4" t="s">
         <v>100</v>
       </c>
@@ -3287,7 +3301,7 @@
       <c r="B78" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C78" s="30"/>
+      <c r="C78" s="27"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4" t="s">
         <v>174</v>
@@ -3305,7 +3319,7 @@
       <c r="B79" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C79" s="30"/>
+      <c r="C79" s="27"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4" t="s">
         <v>54</v>
@@ -3323,7 +3337,7 @@
       <c r="B80" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C80" s="30"/>
+      <c r="C80" s="27"/>
       <c r="D80" s="4" t="s">
         <v>107</v>
       </c>
@@ -3347,7 +3361,7 @@
       <c r="B81" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C81" s="30"/>
+      <c r="C81" s="27"/>
       <c r="D81" s="4" t="s">
         <v>100</v>
       </c>
@@ -3367,7 +3381,7 @@
       <c r="B82" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C82" s="30"/>
+      <c r="C82" s="27"/>
       <c r="D82" s="4" t="s">
         <v>179</v>
       </c>
@@ -3391,7 +3405,7 @@
       <c r="B83" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C83" s="30"/>
+      <c r="C83" s="27"/>
       <c r="D83" s="4" t="s">
         <v>182</v>
       </c>
@@ -3415,7 +3429,7 @@
       <c r="B84" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C84" s="30"/>
+      <c r="C84" s="27"/>
       <c r="D84" s="4" t="s">
         <v>185</v>
       </c>
@@ -3439,7 +3453,7 @@
       <c r="B85" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C85" s="30"/>
+      <c r="C85" s="27"/>
       <c r="D85" s="4" t="s">
         <v>188</v>
       </c>
@@ -3463,7 +3477,7 @@
       <c r="B86" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C86" s="30"/>
+      <c r="C86" s="27"/>
       <c r="D86" s="4" t="s">
         <v>192</v>
       </c>
@@ -3487,7 +3501,7 @@
       <c r="B87" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C87" s="30"/>
+      <c r="C87" s="27"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4" t="s">
         <v>194</v>
@@ -3505,7 +3519,7 @@
       <c r="B88" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C88" s="30"/>
+      <c r="C88" s="27"/>
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
         <v>77</v>
@@ -3523,7 +3537,7 @@
       <c r="B89" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C89" s="31"/>
+      <c r="C89" s="28"/>
       <c r="D89" s="4" t="s">
         <v>195</v>
       </c>
@@ -3541,16 +3555,16 @@
       </c>
     </row>
     <row r="90" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="32" t="s">
+      <c r="A90" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="B90" s="33"/>
-      <c r="C90" s="33"/>
-      <c r="D90" s="33"/>
-      <c r="E90" s="33"/>
-      <c r="F90" s="33"/>
-      <c r="G90" s="33"/>
-      <c r="H90" s="34"/>
+      <c r="B90" s="30"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="30"/>
+      <c r="F90" s="30"/>
+      <c r="G90" s="30"/>
+      <c r="H90" s="31"/>
     </row>
     <row r="91" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
@@ -3559,7 +3573,7 @@
       <c r="B91" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C91" s="29" t="s">
+      <c r="C91" s="26" t="s">
         <v>282</v>
       </c>
       <c r="D91" s="4" t="s">
@@ -3585,7 +3599,7 @@
       <c r="B92" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C92" s="30"/>
+      <c r="C92" s="27"/>
       <c r="D92" s="4" t="s">
         <v>203</v>
       </c>
@@ -3605,7 +3619,7 @@
       <c r="B93" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C93" s="30"/>
+      <c r="C93" s="27"/>
       <c r="D93" s="4" t="s">
         <v>205</v>
       </c>
@@ -3625,7 +3639,7 @@
       <c r="B94" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="C94" s="30"/>
+      <c r="C94" s="27"/>
       <c r="D94" s="4" t="s">
         <v>207</v>
       </c>
@@ -3645,7 +3659,7 @@
       <c r="B95" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C95" s="30"/>
+      <c r="C95" s="27"/>
       <c r="D95" s="4" t="s">
         <v>209</v>
       </c>
@@ -3665,7 +3679,7 @@
       <c r="B96" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="C96" s="30"/>
+      <c r="C96" s="27"/>
       <c r="D96" s="4" t="s">
         <v>211</v>
       </c>
@@ -3689,7 +3703,7 @@
       <c r="B97" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C97" s="30"/>
+      <c r="C97" s="27"/>
       <c r="D97" s="4" t="s">
         <v>214</v>
       </c>
@@ -3713,7 +3727,7 @@
       <c r="B98" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C98" s="30"/>
+      <c r="C98" s="27"/>
       <c r="D98" s="4" t="s">
         <v>217</v>
       </c>
@@ -3737,7 +3751,7 @@
       <c r="B99" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="C99" s="30"/>
+      <c r="C99" s="27"/>
       <c r="D99" s="4" t="s">
         <v>220</v>
       </c>
@@ -3761,7 +3775,7 @@
       <c r="B100" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C100" s="30"/>
+      <c r="C100" s="27"/>
       <c r="D100" s="4">
         <v>12345678</v>
       </c>
@@ -3785,7 +3799,7 @@
       <c r="B101" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="C101" s="30"/>
+      <c r="C101" s="27"/>
       <c r="D101" s="4" t="s">
         <v>225</v>
       </c>
@@ -3809,7 +3823,7 @@
       <c r="B102" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C102" s="30"/>
+      <c r="C102" s="27"/>
       <c r="D102" s="4" t="s">
         <v>228</v>
       </c>
@@ -3833,7 +3847,7 @@
       <c r="B103" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C103" s="30"/>
+      <c r="C103" s="27"/>
       <c r="D103" s="4"/>
       <c r="E103" s="4" t="s">
         <v>200</v>
@@ -3855,7 +3869,7 @@
       <c r="B104" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C104" s="30"/>
+      <c r="C104" s="27"/>
       <c r="D104" s="4" t="s">
         <v>233</v>
       </c>
@@ -3879,7 +3893,7 @@
       <c r="B105" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C105" s="30"/>
+      <c r="C105" s="27"/>
       <c r="D105" s="4" t="s">
         <v>236</v>
       </c>
@@ -3903,7 +3917,7 @@
       <c r="B106" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C106" s="30"/>
+      <c r="C106" s="27"/>
       <c r="D106" s="4" t="s">
         <v>239</v>
       </c>
@@ -3927,7 +3941,7 @@
       <c r="B107" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="C107" s="30"/>
+      <c r="C107" s="27"/>
       <c r="D107" s="4" t="s">
         <v>242</v>
       </c>
@@ -3951,7 +3965,7 @@
       <c r="B108" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C108" s="30"/>
+      <c r="C108" s="27"/>
       <c r="D108" s="4" t="s">
         <v>245</v>
       </c>
@@ -3971,7 +3985,7 @@
       <c r="B109" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="C109" s="30"/>
+      <c r="C109" s="27"/>
       <c r="D109" s="4" t="s">
         <v>245</v>
       </c>
@@ -3991,7 +4005,7 @@
       <c r="B110" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C110" s="30"/>
+      <c r="C110" s="27"/>
       <c r="D110" s="4" t="s">
         <v>245</v>
       </c>
@@ -4011,7 +4025,7 @@
       <c r="B111" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C111" s="30"/>
+      <c r="C111" s="27"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4" t="s">
         <v>75</v>
@@ -4029,7 +4043,7 @@
       <c r="B112" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C112" s="30"/>
+      <c r="C112" s="27"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4" t="s">
         <v>77</v>
@@ -4047,7 +4061,7 @@
       <c r="B113" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C113" s="30"/>
+      <c r="C113" s="27"/>
       <c r="D113" s="4"/>
       <c r="E113" s="9" t="s">
         <v>174</v>
@@ -4065,7 +4079,7 @@
       <c r="B114" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C114" s="30"/>
+      <c r="C114" s="27"/>
       <c r="D114" s="2"/>
       <c r="E114" s="12" t="s">
         <v>54</v>
@@ -4083,7 +4097,7 @@
       <c r="B115" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C115" s="31"/>
+      <c r="C115" s="28"/>
       <c r="D115" s="4" t="s">
         <v>249</v>
       </c>
@@ -7263,7 +7277,7 @@
   <customSheetViews>
     <customSheetView guid="{0B523258-5331-49A5-8E12-7693DC3B142F}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:B11" xr:uid="{42C76EB5-83CE-421F-ACC2-328E68B003D7}"/>
+      <autoFilter ref="A2:B11" xr:uid="{934709D3-52E3-4C6E-9BB2-53D0DC2788AC}"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -7279,7 +7293,7 @@
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7288,36 +7302,36 @@
     <col min="2" max="26" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20"/>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="37" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="A4" s="27"/>
     </row>
     <row r="5" spans="1:1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+      <c r="A5" s="27"/>
     </row>
     <row r="6" spans="1:1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="27"/>
     </row>
     <row r="7" spans="1:1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="27"/>
     </row>
     <row r="8" spans="1:1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-    </row>
-    <row r="9" spans="1:1" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A8" s="27"/>
+    </row>
+    <row r="9" spans="1:1" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
     </row>
     <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>